<commit_message>
I finished the project "Extract_invoice_details_Web_Site"
</commit_message>
<xml_diff>
--- a/Output_Files/out_VendorID_Input.xlsx
+++ b/Output_Files/out_VendorID_Input.xlsx
@@ -1,97 +1,113 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganga.y\Downloads\Exercise_Input_Output_Activities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\test\Documents\Github RPA\RPA_Training_Tutorials\Output_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A8BF59-E307-4BBB-98FA-68EB3A62624C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B12FEA-BE8C-48D7-9468-370CDECE1CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="162913"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Invoice Number</t>
-  </si>
-  <si>
-    <t>Vendor Tax ID</t>
-  </si>
-  <si>
-    <t>Invoice Item</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>Invoice Number</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vendor Tax ID</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Invoice Item</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Total</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Date</x:t>
+  </x:si>
+  <x:si>
+    <x:t>was found?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Not Found</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,64 +372,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="19.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>494559</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>815068</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>845135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>642745</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>622888</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{00000000-0001-0000-0000-000000000000}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F6"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="F2" sqref="F2 F2:F6"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultColWidth="17.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <x:cols>
+    <x:col min="1" max="1" width="19.664062" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="13.441406" style="0" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="29.109375" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="A2" s="0">
+        <x:v>494559</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="A3" s="0">
+        <x:v>815068</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="A4" s="0">
+        <x:v>845135</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="A5" s="0">
+        <x:v>642745</x:v>
+      </x:c>
+      <x:c r="F5" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <x:c r="A6" s="0">
+        <x:v>622888</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>